<commit_message>
Added save feature for 2S modules.
</commit_message>
<xml_diff>
--- a/data/geometry_carbonFoam.xlsx
+++ b/data/geometry_carbonFoam.xlsx
@@ -258,8 +258,8 @@
   </sheetPr>
   <dimension ref="A1:L355"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A300" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A295" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A352" activeCellId="0" sqref="352:352"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5094,33 +5094,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B208" s="1" t="n">
-        <v>692.345405</v>
-      </c>
-      <c r="C208" s="1" t="n">
-        <v>180</v>
-      </c>
-      <c r="D208" s="2" t="n">
-        <v>-6.70000000000005</v>
-      </c>
-      <c r="E208" s="1" t="n">
-        <v>103</v>
-      </c>
-      <c r="F208" s="1" t="n">
-        <v>93</v>
-      </c>
-      <c r="J208" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="K208" s="0" t="n">
-        <f aca="false">IF(ISBLANK(J208), "", $L$2*J208)</f>
-        <v>8</v>
-      </c>
-    </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K209" s="0" t="str">
         <f aca="false">IF(ISBLANK(J209), "", $L$2*J209)</f>
@@ -6034,40 +6007,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B240" s="1" t="n">
-        <v>800.055936</v>
-      </c>
-      <c r="C240" s="1" t="n">
-        <v>180</v>
-      </c>
-      <c r="D240" s="2" t="n">
-        <v>21.6000000000001</v>
-      </c>
-      <c r="E240" s="1" t="n">
-        <v>103</v>
-      </c>
-      <c r="F240" s="1" t="n">
-        <v>93</v>
-      </c>
-      <c r="J240" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="K240" s="0" t="n">
-        <f aca="false">IF(ISBLANK(J240), "", $L$2*J240)</f>
-        <v>8</v>
-      </c>
-    </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H241" s="1" t="s">
         <v>24</v>
       </c>
       <c r="I241" s="1" t="n">
         <f aca="false">B242-B208</f>
-        <v>181.098861</v>
+        <v>873.444266</v>
       </c>
       <c r="K241" s="0" t="str">
         <f aca="false">IF(ISBLANK(J241), "", $L$2*J241)</f>
@@ -7042,33 +6988,6 @@
       </c>
       <c r="K273" s="0" t="n">
         <f aca="false">IF(ISBLANK(J273), "", $L$2*J273)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B274" s="1" t="n">
-        <v>873.444266</v>
-      </c>
-      <c r="C274" s="1" t="n">
-        <v>180</v>
-      </c>
-      <c r="D274" s="2" t="n">
-        <v>-6.70000000000005</v>
-      </c>
-      <c r="E274" s="1" t="n">
-        <v>103</v>
-      </c>
-      <c r="F274" s="1" t="n">
-        <v>93</v>
-      </c>
-      <c r="J274" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="K274" s="0" t="n">
-        <f aca="false">IF(ISBLANK(J274), "", $L$2*J274)</f>
         <v>8</v>
       </c>
     </row>
@@ -8165,40 +8084,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A312" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B312" s="1" t="n">
-        <v>982.515209</v>
-      </c>
-      <c r="C312" s="1" t="n">
-        <v>180</v>
-      </c>
-      <c r="D312" s="2" t="n">
-        <v>21.6000000000001</v>
-      </c>
-      <c r="E312" s="1" t="n">
-        <v>103</v>
-      </c>
-      <c r="F312" s="1" t="n">
-        <v>93</v>
-      </c>
-      <c r="J312" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="K312" s="0" t="n">
-        <f aca="false">IF(ISBLANK(J312), "", $L$2*J312)</f>
-        <v>8</v>
-      </c>
-    </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H313" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I313" s="1" t="n">
         <f aca="false">B314-B208</f>
-        <v>357.404595</v>
+        <v>1049.75</v>
       </c>
       <c r="K313" s="0" t="str">
         <f aca="false">IF(ISBLANK(J313), "", $L$2*J313)</f>
@@ -9353,33 +9245,6 @@
       </c>
       <c r="K351" s="0" t="n">
         <f aca="false">IF(ISBLANK(J351), "", $L$2*J351)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A352" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B352" s="1" t="n">
-        <v>1049.75</v>
-      </c>
-      <c r="C352" s="1" t="n">
-        <v>180</v>
-      </c>
-      <c r="D352" s="2" t="n">
-        <v>-6.70000000000005</v>
-      </c>
-      <c r="E352" s="1" t="n">
-        <v>103</v>
-      </c>
-      <c r="F352" s="1" t="n">
-        <v>93</v>
-      </c>
-      <c r="J352" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="K352" s="0" t="n">
-        <f aca="false">IF(ISBLANK(J352), "", $L$2*J352)</f>
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New features and bug fixes.
</commit_message>
<xml_diff>
--- a/data/geometry_carbonFoam.xlsx
+++ b/data/geometry_carbonFoam.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="13">
   <si>
     <t xml:space="preserve"> Ring</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve"> length(mm) (radial)</t>
   </si>
   <si>
+    <t xml:space="preserve">side</t>
+  </si>
+  <si>
     <t xml:space="preserve">insert outer radius (mm) (actual)</t>
   </si>
   <si>
@@ -52,55 +55,10 @@
     <t xml:space="preserve">46.26</t>
   </si>
   <si>
-    <t xml:space="preserve">_frst</t>
+    <t xml:space="preserve">top</t>
   </si>
   <si>
-    <t xml:space="preserve">_shrt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Steigung:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_long</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offset(3-1):</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offset(5-3):</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offset(5-1):</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Steigungswinkel:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offset(7-1):</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offset(9-1):</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_shlo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_losh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_sh90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offset(11-13):</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_lo90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offset(15-11):</t>
+    <t xml:space="preserve">bottom</t>
   </si>
 </sst>
 </file>
@@ -209,21 +167,21 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -231,10 +189,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -258,8 +220,8 @@
   </sheetPr>
   <dimension ref="A1:L355"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A295" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A352" activeCellId="0" sqref="352:352"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -270,9 +232,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="28.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="32.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="12" style="0" width="8.8"/>
@@ -298,14 +260,17 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="J1" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -325,9 +290,6 @@
         <v>96</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L2" s="0" t="n">
@@ -351,17 +313,7 @@
         <v>96</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <f aca="false">C4-C2</f>
-        <v>36</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -381,10 +333,7 @@
         <v>96</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -406,9 +355,6 @@
       <c r="F5" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -429,9 +375,6 @@
       <c r="F6" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -452,9 +395,6 @@
       <c r="F7" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -475,9 +415,6 @@
       <c r="F8" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -498,9 +435,6 @@
       <c r="F9" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -521,9 +455,6 @@
       <c r="F10" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -544,29 +475,6 @@
       <c r="F11" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B12" s="1" t="n">
-        <v>252.270376</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>180</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>-6.73000000000002</v>
-      </c>
-      <c r="E12" s="1" t="n">
-        <v>96</v>
-      </c>
-      <c r="F12" s="1" t="n">
-        <v>46.26</v>
-      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -587,9 +495,6 @@
       <c r="F14" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -610,16 +515,6 @@
       <c r="F15" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I15" s="1" t="n">
-        <f aca="false">C16-C14</f>
-        <v>30</v>
-      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -640,9 +535,6 @@
       <c r="F16" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -663,9 +555,6 @@
       <c r="F17" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -686,9 +575,6 @@
       <c r="F18" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -709,9 +595,6 @@
       <c r="F19" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -732,9 +615,6 @@
       <c r="F20" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -755,9 +635,6 @@
       <c r="F21" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -778,9 +655,6 @@
       <c r="F22" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -801,9 +675,6 @@
       <c r="F23" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -824,9 +695,6 @@
       <c r="F24" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
@@ -847,9 +715,6 @@
       <c r="F25" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
@@ -878,7 +743,7 @@
       <c r="B28" s="1" t="n">
         <v>338.197069</v>
       </c>
-      <c r="C28" s="3" t="n">
+      <c r="C28" s="1" t="n">
         <v>7.5</v>
       </c>
       <c r="D28" s="2" t="n">
@@ -889,16 +754,6 @@
       </c>
       <c r="F28" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I28" s="1" t="n">
-        <f aca="false">B28-B12</f>
-        <v>85.926693</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -908,7 +763,7 @@
       <c r="B29" s="1" t="n">
         <v>338.197069</v>
       </c>
-      <c r="C29" s="3" t="n">
+      <c r="C29" s="1" t="n">
         <v>22.5</v>
       </c>
       <c r="D29" s="2" t="n">
@@ -919,16 +774,6 @@
       </c>
       <c r="F29" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I29" s="1" t="n">
-        <f aca="false">C30-C28</f>
-        <v>30</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -938,7 +783,7 @@
       <c r="B30" s="1" t="n">
         <v>338.197069</v>
       </c>
-      <c r="C30" s="3" t="n">
+      <c r="C30" s="1" t="n">
         <v>37.5</v>
       </c>
       <c r="D30" s="2" t="n">
@@ -949,9 +794,6 @@
       </c>
       <c r="F30" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -961,7 +803,7 @@
       <c r="B31" s="1" t="n">
         <v>338.197069</v>
       </c>
-      <c r="C31" s="3" t="n">
+      <c r="C31" s="1" t="n">
         <v>52.5</v>
       </c>
       <c r="D31" s="2" t="n">
@@ -972,9 +814,6 @@
       </c>
       <c r="F31" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -984,7 +823,7 @@
       <c r="B32" s="1" t="n">
         <v>338.197069</v>
       </c>
-      <c r="C32" s="3" t="n">
+      <c r="C32" s="1" t="n">
         <v>67.5</v>
       </c>
       <c r="D32" s="2" t="n">
@@ -995,9 +834,6 @@
       </c>
       <c r="F32" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1007,7 +843,7 @@
       <c r="B33" s="1" t="n">
         <v>338.197069</v>
       </c>
-      <c r="C33" s="3" t="n">
+      <c r="C33" s="1" t="n">
         <v>82.5</v>
       </c>
       <c r="D33" s="2" t="n">
@@ -1018,9 +854,6 @@
       </c>
       <c r="F33" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1030,7 +863,7 @@
       <c r="B34" s="1" t="n">
         <v>338.197069</v>
       </c>
-      <c r="C34" s="3" t="n">
+      <c r="C34" s="1" t="n">
         <v>97.5</v>
       </c>
       <c r="D34" s="2" t="n">
@@ -1041,9 +874,6 @@
       </c>
       <c r="F34" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1053,7 +883,7 @@
       <c r="B35" s="1" t="n">
         <v>338.197069</v>
       </c>
-      <c r="C35" s="3" t="n">
+      <c r="C35" s="1" t="n">
         <v>112.5</v>
       </c>
       <c r="D35" s="2" t="n">
@@ -1064,9 +894,6 @@
       </c>
       <c r="F35" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,7 +903,7 @@
       <c r="B36" s="1" t="n">
         <v>338.197069</v>
       </c>
-      <c r="C36" s="3" t="n">
+      <c r="C36" s="1" t="n">
         <v>127.5</v>
       </c>
       <c r="D36" s="2" t="n">
@@ -1087,9 +914,6 @@
       </c>
       <c r="F36" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1099,7 +923,7 @@
       <c r="B37" s="1" t="n">
         <v>338.197069</v>
       </c>
-      <c r="C37" s="3" t="n">
+      <c r="C37" s="1" t="n">
         <v>142.5</v>
       </c>
       <c r="D37" s="2" t="n">
@@ -1110,9 +934,6 @@
       </c>
       <c r="F37" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1122,7 +943,7 @@
       <c r="B38" s="1" t="n">
         <v>338.197069</v>
       </c>
-      <c r="C38" s="3" t="n">
+      <c r="C38" s="1" t="n">
         <v>157.5</v>
       </c>
       <c r="D38" s="2" t="n">
@@ -1133,9 +954,6 @@
       </c>
       <c r="F38" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1145,7 +963,7 @@
       <c r="B39" s="1" t="n">
         <v>338.197069</v>
       </c>
-      <c r="C39" s="3" t="n">
+      <c r="C39" s="1" t="n">
         <v>172.5</v>
       </c>
       <c r="D39" s="2" t="n">
@@ -1157,29 +975,6 @@
       <c r="F39" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B40" s="1" t="n">
-        <v>338.197069</v>
-      </c>
-      <c r="C40" s="1" t="n">
-        <v>180</v>
-      </c>
-      <c r="D40" s="2" t="n">
-        <v>-6.73000000000002</v>
-      </c>
-      <c r="E40" s="1" t="n">
-        <v>96</v>
-      </c>
-      <c r="F40" s="1" t="n">
-        <v>46.26</v>
-      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
@@ -1200,9 +995,6 @@
       <c r="F42" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
@@ -1223,16 +1015,6 @@
       <c r="F43" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G43" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I43" s="1" t="n">
-        <f aca="false">C44-C42</f>
-        <v>25.714286</v>
-      </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
@@ -1253,9 +1035,6 @@
       <c r="F44" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
@@ -1276,9 +1055,6 @@
       <c r="F45" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
@@ -1299,9 +1075,6 @@
       <c r="F46" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
@@ -1322,9 +1095,6 @@
       <c r="F47" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G47" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
@@ -1345,9 +1115,6 @@
       <c r="F48" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G48" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
@@ -1368,9 +1135,6 @@
       <c r="F49" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G49" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
@@ -1391,9 +1155,6 @@
       <c r="F50" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G50" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
@@ -1414,9 +1175,6 @@
       <c r="F51" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G51" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
@@ -1437,9 +1195,6 @@
       <c r="F52" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G52" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
@@ -1460,9 +1215,6 @@
       <c r="F53" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G53" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
@@ -1483,9 +1235,6 @@
       <c r="F54" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G54" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
@@ -1506,9 +1255,6 @@
       <c r="F55" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G55" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
@@ -1528,15 +1274,6 @@
       </c>
       <c r="F56" s="1" t="n">
         <v>46.26</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H57" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I57" s="1" t="n">
-        <f aca="false">B58-B40</f>
-        <v>83.400853</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1546,7 +1283,7 @@
       <c r="B58" s="1" t="n">
         <v>421.597922</v>
       </c>
-      <c r="C58" s="3" t="n">
+      <c r="C58" s="1" t="n">
         <v>5.625</v>
       </c>
       <c r="D58" s="2" t="n">
@@ -1557,16 +1294,6 @@
       </c>
       <c r="F58" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I58" s="1" t="n">
-        <f aca="false">B58-B12</f>
-        <v>169.327546</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1576,7 +1303,7 @@
       <c r="B59" s="1" t="n">
         <v>421.597922</v>
       </c>
-      <c r="C59" s="3" t="n">
+      <c r="C59" s="1" t="n">
         <v>16.875</v>
       </c>
       <c r="D59" s="2" t="n">
@@ -1587,16 +1314,6 @@
       </c>
       <c r="F59" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I59" s="1" t="n">
-        <f aca="false">C60-C58</f>
-        <v>22.5</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1606,7 +1323,7 @@
       <c r="B60" s="1" t="n">
         <v>421.597922</v>
       </c>
-      <c r="C60" s="3" t="n">
+      <c r="C60" s="1" t="n">
         <v>28.125</v>
       </c>
       <c r="D60" s="2" t="n">
@@ -1617,9 +1334,6 @@
       </c>
       <c r="F60" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1629,7 +1343,7 @@
       <c r="B61" s="1" t="n">
         <v>421.597922</v>
       </c>
-      <c r="C61" s="3" t="n">
+      <c r="C61" s="1" t="n">
         <v>39.375</v>
       </c>
       <c r="D61" s="2" t="n">
@@ -1640,9 +1354,6 @@
       </c>
       <c r="F61" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1652,7 +1363,7 @@
       <c r="B62" s="1" t="n">
         <v>421.597922</v>
       </c>
-      <c r="C62" s="3" t="n">
+      <c r="C62" s="1" t="n">
         <v>50.625</v>
       </c>
       <c r="D62" s="2" t="n">
@@ -1663,9 +1374,6 @@
       </c>
       <c r="F62" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1675,7 +1383,7 @@
       <c r="B63" s="1" t="n">
         <v>421.597922</v>
       </c>
-      <c r="C63" s="3" t="n">
+      <c r="C63" s="1" t="n">
         <v>61.875</v>
       </c>
       <c r="D63" s="2" t="n">
@@ -1686,9 +1394,6 @@
       </c>
       <c r="F63" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1698,7 +1403,7 @@
       <c r="B64" s="1" t="n">
         <v>421.597922</v>
       </c>
-      <c r="C64" s="3" t="n">
+      <c r="C64" s="1" t="n">
         <v>73.125</v>
       </c>
       <c r="D64" s="2" t="n">
@@ -1709,9 +1414,6 @@
       </c>
       <c r="F64" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1721,7 +1423,7 @@
       <c r="B65" s="1" t="n">
         <v>421.597922</v>
       </c>
-      <c r="C65" s="3" t="n">
+      <c r="C65" s="1" t="n">
         <v>84.375</v>
       </c>
       <c r="D65" s="2" t="n">
@@ -1732,9 +1434,6 @@
       </c>
       <c r="F65" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1744,7 +1443,7 @@
       <c r="B66" s="1" t="n">
         <v>421.597922</v>
       </c>
-      <c r="C66" s="3" t="n">
+      <c r="C66" s="1" t="n">
         <v>95.625</v>
       </c>
       <c r="D66" s="2" t="n">
@@ -1755,9 +1454,6 @@
       </c>
       <c r="F66" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1767,7 +1463,7 @@
       <c r="B67" s="1" t="n">
         <v>421.597922</v>
       </c>
-      <c r="C67" s="3" t="n">
+      <c r="C67" s="1" t="n">
         <v>106.875</v>
       </c>
       <c r="D67" s="2" t="n">
@@ -1778,9 +1474,6 @@
       </c>
       <c r="F67" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,7 +1483,7 @@
       <c r="B68" s="1" t="n">
         <v>421.597922</v>
       </c>
-      <c r="C68" s="3" t="n">
+      <c r="C68" s="1" t="n">
         <v>118.125</v>
       </c>
       <c r="D68" s="2" t="n">
@@ -1801,9 +1494,6 @@
       </c>
       <c r="F68" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1813,7 +1503,7 @@
       <c r="B69" s="1" t="n">
         <v>421.597922</v>
       </c>
-      <c r="C69" s="3" t="n">
+      <c r="C69" s="1" t="n">
         <v>129.375</v>
       </c>
       <c r="D69" s="2" t="n">
@@ -1824,9 +1514,6 @@
       </c>
       <c r="F69" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1836,7 +1523,7 @@
       <c r="B70" s="1" t="n">
         <v>421.597922</v>
       </c>
-      <c r="C70" s="3" t="n">
+      <c r="C70" s="1" t="n">
         <v>140.625</v>
       </c>
       <c r="D70" s="2" t="n">
@@ -1847,9 +1534,6 @@
       </c>
       <c r="F70" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1859,7 +1543,7 @@
       <c r="B71" s="1" t="n">
         <v>421.597922</v>
       </c>
-      <c r="C71" s="3" t="n">
+      <c r="C71" s="1" t="n">
         <v>151.875</v>
       </c>
       <c r="D71" s="2" t="n">
@@ -1870,9 +1554,6 @@
       </c>
       <c r="F71" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1882,7 +1563,7 @@
       <c r="B72" s="1" t="n">
         <v>421.597922</v>
       </c>
-      <c r="C72" s="3" t="n">
+      <c r="C72" s="1" t="n">
         <v>163.125</v>
       </c>
       <c r="D72" s="2" t="n">
@@ -1893,9 +1574,6 @@
       </c>
       <c r="F72" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1905,7 +1583,7 @@
       <c r="B73" s="1" t="n">
         <v>421.597922</v>
       </c>
-      <c r="C73" s="3" t="n">
+      <c r="C73" s="1" t="n">
         <v>174.375</v>
       </c>
       <c r="D73" s="2" t="n">
@@ -1915,29 +1593,6 @@
         <v>96</v>
       </c>
       <c r="F73" s="1" t="n">
-        <v>46.26</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B74" s="1" t="n">
-        <v>421.597922</v>
-      </c>
-      <c r="C74" s="1" t="n">
-        <v>180</v>
-      </c>
-      <c r="D74" s="2" t="n">
-        <v>-6.73000000000002</v>
-      </c>
-      <c r="E74" s="1" t="n">
-        <v>96</v>
-      </c>
-      <c r="F74" s="1" t="n">
         <v>46.26</v>
       </c>
     </row>
@@ -1960,9 +1615,6 @@
       <c r="F76" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G76" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="n">
@@ -1983,16 +1635,6 @@
       <c r="F77" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G77" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H77" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I77" s="1" t="n">
-        <f aca="false">C78-C76</f>
-        <v>22.5</v>
-      </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="n">
@@ -2013,9 +1655,6 @@
       <c r="F78" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G78" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="n">
@@ -2036,9 +1675,6 @@
       <c r="F79" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G79" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="n">
@@ -2059,9 +1695,6 @@
       <c r="F80" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G80" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="n">
@@ -2082,9 +1715,6 @@
       <c r="F81" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G81" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="n">
@@ -2105,9 +1735,6 @@
       <c r="F82" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G82" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="n">
@@ -2128,9 +1755,6 @@
       <c r="F83" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G83" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="n">
@@ -2151,9 +1775,6 @@
       <c r="F84" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G84" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="n">
@@ -2174,9 +1795,6 @@
       <c r="F85" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G85" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="n">
@@ -2197,9 +1815,6 @@
       <c r="F86" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G86" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="n">
@@ -2220,9 +1835,6 @@
       <c r="F87" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G87" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="n">
@@ -2243,9 +1855,6 @@
       <c r="F88" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G88" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="n">
@@ -2266,9 +1875,6 @@
       <c r="F89" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G89" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="n">
@@ -2289,9 +1895,6 @@
       <c r="F90" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G90" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="n">
@@ -2312,9 +1915,6 @@
       <c r="F91" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G91" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="n">
@@ -2355,16 +1955,6 @@
       <c r="F94" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G94" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H94" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I94" s="1" t="n">
-        <f aca="false">B94-B12</f>
-        <v>250.276809</v>
-      </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="n">
@@ -2385,16 +1975,6 @@
       <c r="F95" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G95" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H95" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I95" s="1" t="n">
-        <f aca="false">C96-C94</f>
-        <v>20</v>
-      </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="n">
@@ -2415,9 +1995,6 @@
       <c r="F96" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G96" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="n">
@@ -2438,9 +2015,6 @@
       <c r="F97" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G97" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="n">
@@ -2461,9 +2035,6 @@
       <c r="F98" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G98" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="n">
@@ -2484,9 +2055,6 @@
       <c r="F99" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G99" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="n">
@@ -2507,9 +2075,6 @@
       <c r="F100" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G100" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="n">
@@ -2530,9 +2095,6 @@
       <c r="F101" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G101" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="n">
@@ -2553,9 +2115,6 @@
       <c r="F102" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G102" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="n">
@@ -2576,9 +2135,6 @@
       <c r="F103" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G103" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="n">
@@ -2599,9 +2155,6 @@
       <c r="F104" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G104" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="n">
@@ -2622,9 +2175,6 @@
       <c r="F105" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G105" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="n">
@@ -2645,9 +2195,6 @@
       <c r="F106" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G106" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="n">
@@ -2668,9 +2215,6 @@
       <c r="F107" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G107" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="n">
@@ -2691,9 +2235,6 @@
       <c r="F108" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G108" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="n">
@@ -2714,9 +2255,6 @@
       <c r="F109" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G109" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="n">
@@ -2737,9 +2275,6 @@
       <c r="F110" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G110" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="n">
@@ -2760,29 +2295,6 @@
       <c r="F111" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G111" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B112" s="1" t="n">
-        <v>502.547185</v>
-      </c>
-      <c r="C112" s="1" t="n">
-        <v>180</v>
-      </c>
-      <c r="D112" s="2" t="n">
-        <v>-6.73000000000002</v>
-      </c>
-      <c r="E112" s="1" t="n">
-        <v>96</v>
-      </c>
-      <c r="F112" s="1" t="n">
-        <v>46.26</v>
-      </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="n">
@@ -2803,9 +2315,6 @@
       <c r="F114" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G114" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="n">
@@ -2826,16 +2335,6 @@
       <c r="F115" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G115" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H115" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I115" s="1" t="n">
-        <f aca="false">C116-C114</f>
-        <v>18</v>
-      </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="n">
@@ -2856,9 +2355,6 @@
       <c r="F116" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G116" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="n">
@@ -2879,9 +2375,6 @@
       <c r="F117" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G117" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="n">
@@ -2902,9 +2395,6 @@
       <c r="F118" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G118" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="n">
@@ -2925,9 +2415,6 @@
       <c r="F119" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G119" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="n">
@@ -2948,9 +2435,6 @@
       <c r="F120" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G120" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="n">
@@ -2971,9 +2455,6 @@
       <c r="F121" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G121" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="n">
@@ -2994,9 +2475,6 @@
       <c r="F122" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G122" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="n">
@@ -3017,9 +2495,6 @@
       <c r="F123" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G123" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="n">
@@ -3040,9 +2515,6 @@
       <c r="F124" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G124" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="n">
@@ -3063,9 +2535,6 @@
       <c r="F125" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G125" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="n">
@@ -3086,9 +2555,6 @@
       <c r="F126" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G126" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="n">
@@ -3109,9 +2575,6 @@
       <c r="F127" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G127" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="n">
@@ -3132,9 +2595,6 @@
       <c r="F128" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G128" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="n">
@@ -3155,9 +2615,6 @@
       <c r="F129" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G129" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="n">
@@ -3178,9 +2635,6 @@
       <c r="F130" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G130" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="n">
@@ -3201,9 +2655,6 @@
       <c r="F131" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G131" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="n">
@@ -3224,9 +2675,6 @@
       <c r="F132" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G132" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="n">
@@ -3247,9 +2695,6 @@
       <c r="F133" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G133" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="n">
@@ -3269,15 +2714,6 @@
       </c>
       <c r="F134" s="1" t="n">
         <v>46.26</v>
-      </c>
-    </row>
-    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H135" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I135" s="1" t="n">
-        <f aca="false">B136-B12</f>
-        <v>328.846545</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3287,7 +2723,7 @@
       <c r="B136" s="1" t="n">
         <v>581.116921</v>
       </c>
-      <c r="C136" s="3" t="n">
+      <c r="C136" s="1" t="n">
         <v>4.5</v>
       </c>
       <c r="D136" s="2" t="n">
@@ -3298,12 +2734,6 @@
       </c>
       <c r="F136" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G136" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H136" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3313,7 +2743,7 @@
       <c r="B137" s="1" t="n">
         <v>581.116921</v>
       </c>
-      <c r="C137" s="3" t="n">
+      <c r="C137" s="1" t="n">
         <v>13.5</v>
       </c>
       <c r="D137" s="2" t="n">
@@ -3324,16 +2754,6 @@
       </c>
       <c r="F137" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G137" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H137" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I137" s="1" t="n">
-        <f aca="false">C138-C136</f>
-        <v>18</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3343,7 +2763,7 @@
       <c r="B138" s="1" t="n">
         <v>581.116921</v>
       </c>
-      <c r="C138" s="3" t="n">
+      <c r="C138" s="1" t="n">
         <v>22.5</v>
       </c>
       <c r="D138" s="2" t="n">
@@ -3354,9 +2774,6 @@
       </c>
       <c r="F138" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G138" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3366,7 +2783,7 @@
       <c r="B139" s="1" t="n">
         <v>581.116921</v>
       </c>
-      <c r="C139" s="3" t="n">
+      <c r="C139" s="1" t="n">
         <v>31.5</v>
       </c>
       <c r="D139" s="2" t="n">
@@ -3377,9 +2794,6 @@
       </c>
       <c r="F139" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G139" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3389,7 +2803,7 @@
       <c r="B140" s="1" t="n">
         <v>581.116921</v>
       </c>
-      <c r="C140" s="3" t="n">
+      <c r="C140" s="1" t="n">
         <v>40.5</v>
       </c>
       <c r="D140" s="2" t="n">
@@ -3400,9 +2814,6 @@
       </c>
       <c r="F140" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G140" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3412,7 +2823,7 @@
       <c r="B141" s="1" t="n">
         <v>581.116921</v>
       </c>
-      <c r="C141" s="3" t="n">
+      <c r="C141" s="1" t="n">
         <v>49.5</v>
       </c>
       <c r="D141" s="2" t="n">
@@ -3423,9 +2834,6 @@
       </c>
       <c r="F141" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G141" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3435,7 +2843,7 @@
       <c r="B142" s="1" t="n">
         <v>581.116921</v>
       </c>
-      <c r="C142" s="3" t="n">
+      <c r="C142" s="1" t="n">
         <v>58.5</v>
       </c>
       <c r="D142" s="2" t="n">
@@ -3446,9 +2854,6 @@
       </c>
       <c r="F142" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G142" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3458,7 +2863,7 @@
       <c r="B143" s="1" t="n">
         <v>581.116921</v>
       </c>
-      <c r="C143" s="3" t="n">
+      <c r="C143" s="1" t="n">
         <v>67.5</v>
       </c>
       <c r="D143" s="2" t="n">
@@ -3469,9 +2874,6 @@
       </c>
       <c r="F143" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G143" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3481,7 +2883,7 @@
       <c r="B144" s="1" t="n">
         <v>581.116921</v>
       </c>
-      <c r="C144" s="3" t="n">
+      <c r="C144" s="1" t="n">
         <v>76.5</v>
       </c>
       <c r="D144" s="2" t="n">
@@ -3492,9 +2894,6 @@
       </c>
       <c r="F144" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G144" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3504,7 +2903,7 @@
       <c r="B145" s="1" t="n">
         <v>581.116921</v>
       </c>
-      <c r="C145" s="3" t="n">
+      <c r="C145" s="1" t="n">
         <v>85.5</v>
       </c>
       <c r="D145" s="2" t="n">
@@ -3515,9 +2914,6 @@
       </c>
       <c r="F145" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G145" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3527,7 +2923,7 @@
       <c r="B146" s="1" t="n">
         <v>581.116921</v>
       </c>
-      <c r="C146" s="3" t="n">
+      <c r="C146" s="1" t="n">
         <v>94.5</v>
       </c>
       <c r="D146" s="2" t="n">
@@ -3538,9 +2934,6 @@
       </c>
       <c r="F146" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G146" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3550,7 +2943,7 @@
       <c r="B147" s="1" t="n">
         <v>581.116921</v>
       </c>
-      <c r="C147" s="3" t="n">
+      <c r="C147" s="1" t="n">
         <v>103.5</v>
       </c>
       <c r="D147" s="2" t="n">
@@ -3561,9 +2954,6 @@
       </c>
       <c r="F147" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G147" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3573,7 +2963,7 @@
       <c r="B148" s="1" t="n">
         <v>581.116921</v>
       </c>
-      <c r="C148" s="3" t="n">
+      <c r="C148" s="1" t="n">
         <v>112.5</v>
       </c>
       <c r="D148" s="2" t="n">
@@ -3584,9 +2974,6 @@
       </c>
       <c r="F148" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G148" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3596,7 +2983,7 @@
       <c r="B149" s="1" t="n">
         <v>581.116921</v>
       </c>
-      <c r="C149" s="3" t="n">
+      <c r="C149" s="1" t="n">
         <v>121.5</v>
       </c>
       <c r="D149" s="2" t="n">
@@ -3607,9 +2994,6 @@
       </c>
       <c r="F149" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G149" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3619,7 +3003,7 @@
       <c r="B150" s="1" t="n">
         <v>581.116921</v>
       </c>
-      <c r="C150" s="3" t="n">
+      <c r="C150" s="1" t="n">
         <v>130.5</v>
       </c>
       <c r="D150" s="2" t="n">
@@ -3630,9 +3014,6 @@
       </c>
       <c r="F150" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G150" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3642,7 +3023,7 @@
       <c r="B151" s="1" t="n">
         <v>581.116921</v>
       </c>
-      <c r="C151" s="3" t="n">
+      <c r="C151" s="1" t="n">
         <v>139.5</v>
       </c>
       <c r="D151" s="2" t="n">
@@ -3653,9 +3034,6 @@
       </c>
       <c r="F151" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G151" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3665,7 +3043,7 @@
       <c r="B152" s="1" t="n">
         <v>581.116921</v>
       </c>
-      <c r="C152" s="3" t="n">
+      <c r="C152" s="1" t="n">
         <v>148.5</v>
       </c>
       <c r="D152" s="2" t="n">
@@ -3676,9 +3054,6 @@
       </c>
       <c r="F152" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G152" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3688,7 +3063,7 @@
       <c r="B153" s="1" t="n">
         <v>581.116921</v>
       </c>
-      <c r="C153" s="3" t="n">
+      <c r="C153" s="1" t="n">
         <v>157.5</v>
       </c>
       <c r="D153" s="2" t="n">
@@ -3699,9 +3074,6 @@
       </c>
       <c r="F153" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G153" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3711,7 +3083,7 @@
       <c r="B154" s="1" t="n">
         <v>581.116921</v>
       </c>
-      <c r="C154" s="3" t="n">
+      <c r="C154" s="1" t="n">
         <v>166.5</v>
       </c>
       <c r="D154" s="2" t="n">
@@ -3722,9 +3094,6 @@
       </c>
       <c r="F154" s="1" t="n">
         <v>46.26</v>
-      </c>
-      <c r="G154" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3734,7 +3103,7 @@
       <c r="B155" s="1" t="n">
         <v>581.116921</v>
       </c>
-      <c r="C155" s="3" t="n">
+      <c r="C155" s="1" t="n">
         <v>175.5</v>
       </c>
       <c r="D155" s="2" t="n">
@@ -3744,29 +3113,6 @@
         <v>96</v>
       </c>
       <c r="F155" s="1" t="n">
-        <v>46.26</v>
-      </c>
-      <c r="G155" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B156" s="1" t="n">
-        <v>581.116921</v>
-      </c>
-      <c r="C156" s="1" t="n">
-        <v>180</v>
-      </c>
-      <c r="D156" s="2" t="n">
-        <v>-6.73000000000002</v>
-      </c>
-      <c r="E156" s="1" t="n">
-        <v>96</v>
-      </c>
-      <c r="F156" s="1" t="n">
         <v>46.26</v>
       </c>
     </row>
@@ -3789,9 +3135,6 @@
       <c r="F158" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G158" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="n">
@@ -3812,16 +3155,6 @@
       <c r="F159" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G159" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H159" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I159" s="1" t="n">
-        <f aca="false">C160-C158</f>
-        <v>16.363636</v>
-      </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="n">
@@ -3842,9 +3175,6 @@
       <c r="F160" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G160" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="n">
@@ -3865,9 +3195,6 @@
       <c r="F161" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G161" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="n">
@@ -3888,9 +3215,6 @@
       <c r="F162" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G162" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="n">
@@ -3911,9 +3235,6 @@
       <c r="F163" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G163" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="n">
@@ -3934,9 +3255,6 @@
       <c r="F164" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G164" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="n">
@@ -3957,9 +3275,6 @@
       <c r="F165" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G165" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="n">
@@ -3980,9 +3295,6 @@
       <c r="F166" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G166" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="n">
@@ -4003,9 +3315,6 @@
       <c r="F167" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G167" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="n">
@@ -4026,9 +3335,6 @@
       <c r="F168" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G168" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="n">
@@ -4049,9 +3355,6 @@
       <c r="F169" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G169" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="n">
@@ -4072,9 +3375,6 @@
       <c r="F170" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G170" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="n">
@@ -4095,9 +3395,6 @@
       <c r="F171" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G171" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="n">
@@ -4118,9 +3415,6 @@
       <c r="F172" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G172" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="n">
@@ -4141,9 +3435,6 @@
       <c r="F173" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G173" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="n">
@@ -4164,9 +3455,6 @@
       <c r="F174" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G174" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="n">
@@ -4187,9 +3475,6 @@
       <c r="F175" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G175" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="n">
@@ -4210,9 +3495,6 @@
       <c r="F176" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G176" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="n">
@@ -4233,9 +3515,6 @@
       <c r="F177" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G177" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="n">
@@ -4256,9 +3535,6 @@
       <c r="F178" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G178" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="n">
@@ -4279,9 +3555,6 @@
       <c r="F179" s="1" t="n">
         <v>46.26</v>
       </c>
-      <c r="G179" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="n">
@@ -4323,7 +3596,7 @@
         <v>93</v>
       </c>
       <c r="G182" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J182" s="0" t="n">
         <v>4</v>
@@ -4353,14 +3626,7 @@
         <v>93</v>
       </c>
       <c r="G183" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H183" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I183" s="1" t="n">
-        <f aca="false">C182-C184</f>
-        <v>-13.846154</v>
+        <v>12</v>
       </c>
       <c r="J183" s="0" t="n">
         <v>4</v>
@@ -4392,10 +3658,7 @@
       <c r="G184" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I184" s="4" t="n">
-        <f aca="false">C185-C183</f>
-        <v>14</v>
-      </c>
+      <c r="I184" s="4"/>
       <c r="J184" s="0" t="n">
         <v>4</v>
       </c>
@@ -4424,7 +3687,7 @@
         <v>93</v>
       </c>
       <c r="G185" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J185" s="0" t="n">
         <v>4</v>
@@ -4454,7 +3717,7 @@
         <v>93</v>
       </c>
       <c r="G186" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="J186" s="0" t="n">
         <v>4</v>
@@ -4484,7 +3747,7 @@
         <v>93</v>
       </c>
       <c r="G187" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J187" s="0" t="n">
         <v>4</v>
@@ -4514,7 +3777,7 @@
         <v>93</v>
       </c>
       <c r="G188" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J188" s="0" t="n">
         <v>4</v>
@@ -4544,7 +3807,7 @@
         <v>93</v>
       </c>
       <c r="G189" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J189" s="0" t="n">
         <v>4</v>
@@ -4574,7 +3837,7 @@
         <v>93</v>
       </c>
       <c r="G190" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="J190" s="0" t="n">
         <v>4</v>
@@ -4604,7 +3867,7 @@
         <v>93</v>
       </c>
       <c r="G191" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J191" s="0" t="n">
         <v>4</v>
@@ -4664,7 +3927,7 @@
         <v>93</v>
       </c>
       <c r="G193" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J193" s="0" t="n">
         <v>4</v>
@@ -4694,7 +3957,7 @@
         <v>93</v>
       </c>
       <c r="G194" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="J194" s="0" t="n">
         <v>4</v>
@@ -4724,7 +3987,7 @@
         <v>93</v>
       </c>
       <c r="G195" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="J195" s="0" t="n">
         <v>4</v>
@@ -4754,7 +4017,7 @@
         <v>93</v>
       </c>
       <c r="G196" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J196" s="0" t="n">
         <v>4</v>
@@ -4784,7 +4047,7 @@
         <v>93</v>
       </c>
       <c r="G197" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J197" s="0" t="n">
         <v>4</v>
@@ -4814,7 +4077,7 @@
         <v>93</v>
       </c>
       <c r="G198" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J198" s="0" t="n">
         <v>4</v>
@@ -4844,7 +4107,7 @@
         <v>93</v>
       </c>
       <c r="G199" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="J199" s="0" t="n">
         <v>4</v>
@@ -4904,7 +4167,7 @@
         <v>93</v>
       </c>
       <c r="G201" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J201" s="0" t="n">
         <v>4</v>
@@ -4964,7 +4227,7 @@
         <v>93</v>
       </c>
       <c r="G203" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="J203" s="0" t="n">
         <v>4</v>
@@ -4994,7 +4257,7 @@
         <v>93</v>
       </c>
       <c r="G204" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J204" s="0" t="n">
         <v>4</v>
@@ -5024,7 +4287,7 @@
         <v>93</v>
       </c>
       <c r="G205" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J205" s="0" t="n">
         <v>4</v>
@@ -5054,7 +4317,7 @@
         <v>93</v>
       </c>
       <c r="G206" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J206" s="0" t="n">
         <v>4</v>
@@ -5084,7 +4347,7 @@
         <v>93</v>
       </c>
       <c r="G207" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J207" s="0" t="n">
         <v>4</v>
@@ -5120,7 +4383,7 @@
         <v>93</v>
       </c>
       <c r="G210" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J210" s="0" t="n">
         <v>4</v>
@@ -5150,13 +4413,6 @@
         <v>93</v>
       </c>
       <c r="G211" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H211" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I211" s="1" t="n">
-        <f aca="false">C212-C210</f>
         <v>12</v>
       </c>
       <c r="J211" s="0" t="n">
@@ -5217,7 +4473,7 @@
         <v>93</v>
       </c>
       <c r="G213" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J213" s="0" t="n">
         <v>4</v>
@@ -5277,7 +4533,7 @@
         <v>93</v>
       </c>
       <c r="G215" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="J215" s="0" t="n">
         <v>4</v>
@@ -5307,7 +4563,7 @@
         <v>93</v>
       </c>
       <c r="G216" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J216" s="0" t="n">
         <v>4</v>
@@ -5337,7 +4593,7 @@
         <v>93</v>
       </c>
       <c r="G217" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J217" s="0" t="n">
         <v>4</v>
@@ -5367,7 +4623,7 @@
         <v>93</v>
       </c>
       <c r="G218" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J218" s="0" t="n">
         <v>4</v>
@@ -5397,7 +4653,7 @@
         <v>93</v>
       </c>
       <c r="G219" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="J219" s="0" t="n">
         <v>4</v>
@@ -5457,7 +4713,7 @@
         <v>93</v>
       </c>
       <c r="G221" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J221" s="0" t="n">
         <v>4</v>
@@ -5517,7 +4773,7 @@
         <v>93</v>
       </c>
       <c r="G223" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J223" s="0" t="n">
         <v>4</v>
@@ -5547,7 +4803,7 @@
         <v>93</v>
       </c>
       <c r="G224" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="J224" s="0" t="n">
         <v>4</v>
@@ -5577,7 +4833,7 @@
         <v>93</v>
       </c>
       <c r="G225" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="J225" s="0" t="n">
         <v>4</v>
@@ -5607,7 +4863,7 @@
         <v>93</v>
       </c>
       <c r="G226" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J226" s="0" t="n">
         <v>4</v>
@@ -5637,7 +4893,7 @@
         <v>93</v>
       </c>
       <c r="G227" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J227" s="0" t="n">
         <v>4</v>
@@ -5667,7 +4923,7 @@
         <v>93</v>
       </c>
       <c r="G228" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J228" s="0" t="n">
         <v>4</v>
@@ -5697,7 +4953,7 @@
         <v>93</v>
       </c>
       <c r="G229" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J229" s="0" t="n">
         <v>4</v>
@@ -5727,7 +4983,7 @@
         <v>93</v>
       </c>
       <c r="G230" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="J230" s="0" t="n">
         <v>4</v>
@@ -5757,7 +5013,7 @@
         <v>93</v>
       </c>
       <c r="G231" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J231" s="0" t="n">
         <v>4</v>
@@ -5817,7 +5073,7 @@
         <v>93</v>
       </c>
       <c r="G233" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J233" s="0" t="n">
         <v>4</v>
@@ -5847,7 +5103,7 @@
         <v>93</v>
       </c>
       <c r="G234" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="J234" s="0" t="n">
         <v>4</v>
@@ -5877,7 +5133,7 @@
         <v>93</v>
       </c>
       <c r="G235" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J235" s="0" t="n">
         <v>4</v>
@@ -5907,7 +5163,7 @@
         <v>93</v>
       </c>
       <c r="G236" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J236" s="0" t="n">
         <v>4</v>
@@ -5937,7 +5193,7 @@
         <v>93</v>
       </c>
       <c r="G237" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J237" s="0" t="n">
         <v>4</v>
@@ -5967,7 +5223,7 @@
         <v>93</v>
       </c>
       <c r="G238" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J238" s="0" t="n">
         <v>4</v>
@@ -5997,7 +5253,7 @@
         <v>93</v>
       </c>
       <c r="G239" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J239" s="0" t="n">
         <v>4</v>
@@ -6008,13 +5264,6 @@
       </c>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H241" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I241" s="1" t="n">
-        <f aca="false">B242-B208</f>
-        <v>873.444266</v>
-      </c>
       <c r="K241" s="0" t="str">
         <f aca="false">IF(ISBLANK(J241), "", $L$2*J241)</f>
         <v/>
@@ -6040,14 +5289,7 @@
         <v>93</v>
       </c>
       <c r="G242" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H242" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I242" s="1" t="n">
-        <f aca="false">C242-C244</f>
-        <v>-11.25</v>
+        <v>11</v>
       </c>
       <c r="J242" s="0" t="n">
         <v>4</v>
@@ -6077,11 +5319,7 @@
         <v>93</v>
       </c>
       <c r="G243" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I243" s="1" t="n">
-        <f aca="false">C243-C245</f>
-        <v>-11.25</v>
+        <v>12</v>
       </c>
       <c r="J243" s="0" t="n">
         <v>4</v>
@@ -6141,7 +5379,7 @@
         <v>93</v>
       </c>
       <c r="G245" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J245" s="0" t="n">
         <v>4</v>
@@ -6201,7 +5439,7 @@
         <v>93</v>
       </c>
       <c r="G247" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="J247" s="0" t="n">
         <v>4</v>
@@ -6231,7 +5469,7 @@
         <v>93</v>
       </c>
       <c r="G248" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J248" s="0" t="n">
         <v>4</v>
@@ -6261,7 +5499,7 @@
         <v>93</v>
       </c>
       <c r="G249" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J249" s="0" t="n">
         <v>4</v>
@@ -6291,7 +5529,7 @@
         <v>93</v>
       </c>
       <c r="G250" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J250" s="0" t="n">
         <v>4</v>
@@ -6321,7 +5559,7 @@
         <v>93</v>
       </c>
       <c r="G251" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J251" s="0" t="n">
         <v>4</v>
@@ -6351,7 +5589,7 @@
         <v>93</v>
       </c>
       <c r="G252" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="J252" s="0" t="n">
         <v>4</v>
@@ -6381,7 +5619,7 @@
         <v>93</v>
       </c>
       <c r="G253" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J253" s="0" t="n">
         <v>4</v>
@@ -6441,7 +5679,7 @@
         <v>93</v>
       </c>
       <c r="G255" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J255" s="0" t="n">
         <v>4</v>
@@ -6501,7 +5739,7 @@
         <v>93</v>
       </c>
       <c r="G257" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="J257" s="0" t="n">
         <v>4</v>
@@ -6531,7 +5769,7 @@
         <v>93</v>
       </c>
       <c r="G258" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="J258" s="0" t="n">
         <v>4</v>
@@ -6561,7 +5799,7 @@
         <v>93</v>
       </c>
       <c r="G259" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J259" s="0" t="n">
         <v>4</v>
@@ -6591,7 +5829,7 @@
         <v>93</v>
       </c>
       <c r="G260" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J260" s="0" t="n">
         <v>4</v>
@@ -6621,7 +5859,7 @@
         <v>93</v>
       </c>
       <c r="G261" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J261" s="0" t="n">
         <v>4</v>
@@ -6651,7 +5889,7 @@
         <v>93</v>
       </c>
       <c r="G262" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J262" s="0" t="n">
         <v>4</v>
@@ -6681,7 +5919,7 @@
         <v>93</v>
       </c>
       <c r="G263" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="J263" s="0" t="n">
         <v>4</v>
@@ -6741,7 +5979,7 @@
         <v>93</v>
       </c>
       <c r="G265" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J265" s="0" t="n">
         <v>4</v>
@@ -6801,7 +6039,7 @@
         <v>93</v>
       </c>
       <c r="G267" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J267" s="0" t="n">
         <v>4</v>
@@ -6831,7 +6069,7 @@
         <v>93</v>
       </c>
       <c r="G268" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="J268" s="0" t="n">
         <v>4</v>
@@ -6861,7 +6099,7 @@
         <v>93</v>
       </c>
       <c r="G269" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J269" s="0" t="n">
         <v>4</v>
@@ -6891,7 +6129,7 @@
         <v>93</v>
       </c>
       <c r="G270" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J270" s="0" t="n">
         <v>4</v>
@@ -6921,7 +6159,7 @@
         <v>93</v>
       </c>
       <c r="G271" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J271" s="0" t="n">
         <v>4</v>
@@ -6951,7 +6189,7 @@
         <v>93</v>
       </c>
       <c r="G272" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J272" s="0" t="n">
         <v>4</v>
@@ -6981,7 +6219,7 @@
         <v>93</v>
       </c>
       <c r="G273" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J273" s="0" t="n">
         <v>4</v>
@@ -7017,7 +6255,7 @@
         <v>93</v>
       </c>
       <c r="G276" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J276" s="0" t="n">
         <v>4</v>
@@ -7047,14 +6285,7 @@
         <v>93</v>
       </c>
       <c r="G277" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H277" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I277" s="1" t="n">
-        <f aca="false">C278-C276</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J277" s="0" t="n">
         <v>4</v>
@@ -7114,7 +6345,7 @@
         <v>93</v>
       </c>
       <c r="G279" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J279" s="0" t="n">
         <v>4</v>
@@ -7174,7 +6405,7 @@
         <v>93</v>
       </c>
       <c r="G281" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="J281" s="0" t="n">
         <v>4</v>
@@ -7204,7 +6435,7 @@
         <v>93</v>
       </c>
       <c r="G282" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J282" s="0" t="n">
         <v>4</v>
@@ -7234,7 +6465,7 @@
         <v>93</v>
       </c>
       <c r="G283" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J283" s="0" t="n">
         <v>4</v>
@@ -7264,7 +6495,7 @@
         <v>93</v>
       </c>
       <c r="G284" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J284" s="0" t="n">
         <v>4</v>
@@ -7294,7 +6525,7 @@
         <v>93</v>
       </c>
       <c r="G285" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J285" s="0" t="n">
         <v>4</v>
@@ -7324,7 +6555,7 @@
         <v>93</v>
       </c>
       <c r="G286" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J286" s="0" t="n">
         <v>4</v>
@@ -7354,7 +6585,7 @@
         <v>93</v>
       </c>
       <c r="G287" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J287" s="0" t="n">
         <v>4</v>
@@ -7384,7 +6615,7 @@
         <v>93</v>
       </c>
       <c r="G288" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="J288" s="0" t="n">
         <v>4</v>
@@ -7414,7 +6645,7 @@
         <v>93</v>
       </c>
       <c r="G289" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J289" s="0" t="n">
         <v>4</v>
@@ -7474,7 +6705,7 @@
         <v>93</v>
       </c>
       <c r="G291" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J291" s="0" t="n">
         <v>4</v>
@@ -7534,7 +6765,7 @@
         <v>93</v>
       </c>
       <c r="G293" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="J293" s="0" t="n">
         <v>4</v>
@@ -7564,7 +6795,7 @@
         <v>93</v>
       </c>
       <c r="G294" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="J294" s="0" t="n">
         <v>4</v>
@@ -7594,7 +6825,7 @@
         <v>93</v>
       </c>
       <c r="G295" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J295" s="0" t="n">
         <v>4</v>
@@ -7624,7 +6855,7 @@
         <v>93</v>
       </c>
       <c r="G296" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J296" s="0" t="n">
         <v>4</v>
@@ -7654,7 +6885,7 @@
         <v>93</v>
       </c>
       <c r="G297" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J297" s="0" t="n">
         <v>4</v>
@@ -7684,7 +6915,7 @@
         <v>93</v>
       </c>
       <c r="G298" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J298" s="0" t="n">
         <v>4</v>
@@ -7714,7 +6945,7 @@
         <v>93</v>
       </c>
       <c r="G299" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="J299" s="0" t="n">
         <v>4</v>
@@ -7774,7 +7005,7 @@
         <v>93</v>
       </c>
       <c r="G301" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J301" s="0" t="n">
         <v>4</v>
@@ -7834,7 +7065,7 @@
         <v>93</v>
       </c>
       <c r="G303" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J303" s="0" t="n">
         <v>4</v>
@@ -7894,7 +7125,7 @@
         <v>93</v>
       </c>
       <c r="G305" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J305" s="0" t="n">
         <v>4</v>
@@ -7924,7 +7155,7 @@
         <v>93</v>
       </c>
       <c r="G306" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="J306" s="0" t="n">
         <v>4</v>
@@ -7954,7 +7185,7 @@
         <v>93</v>
       </c>
       <c r="G307" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J307" s="0" t="n">
         <v>4</v>
@@ -7984,7 +7215,7 @@
         <v>93</v>
       </c>
       <c r="G308" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J308" s="0" t="n">
         <v>4</v>
@@ -8014,7 +7245,7 @@
         <v>93</v>
       </c>
       <c r="G309" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J309" s="0" t="n">
         <v>4</v>
@@ -8044,7 +7275,7 @@
         <v>93</v>
       </c>
       <c r="G310" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J310" s="0" t="n">
         <v>4</v>
@@ -8074,7 +7305,7 @@
         <v>93</v>
       </c>
       <c r="G311" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J311" s="0" t="n">
         <v>4</v>
@@ -8085,13 +7316,6 @@
       </c>
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H313" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I313" s="1" t="n">
-        <f aca="false">B314-B208</f>
-        <v>1049.75</v>
-      </c>
       <c r="K313" s="0" t="str">
         <f aca="false">IF(ISBLANK(J313), "", $L$2*J313)</f>
         <v/>
@@ -8117,14 +7341,7 @@
         <v>93</v>
       </c>
       <c r="G314" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H314" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I314" s="1" t="n">
-        <f aca="false">C314-C316</f>
-        <v>-9.47368400000003</v>
+        <v>11</v>
       </c>
       <c r="J314" s="0" t="n">
         <v>4</v>
@@ -8154,11 +7371,7 @@
         <v>93</v>
       </c>
       <c r="G315" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I315" s="1" t="n">
-        <f aca="false">C315-C317</f>
-        <v>-9.47368400000003</v>
+        <v>12</v>
       </c>
       <c r="J315" s="0" t="n">
         <v>4</v>
@@ -8218,7 +7431,7 @@
         <v>93</v>
       </c>
       <c r="G317" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J317" s="0" t="n">
         <v>4</v>
@@ -8278,7 +7491,7 @@
         <v>93</v>
       </c>
       <c r="G319" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J319" s="0" t="n">
         <v>4</v>
@@ -8308,7 +7521,7 @@
         <v>93</v>
       </c>
       <c r="G320" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="J320" s="0" t="n">
         <v>4</v>
@@ -8338,7 +7551,7 @@
         <v>93</v>
       </c>
       <c r="G321" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J321" s="0" t="n">
         <v>4</v>
@@ -8368,7 +7581,7 @@
         <v>93</v>
       </c>
       <c r="G322" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J322" s="0" t="n">
         <v>4</v>
@@ -8398,7 +7611,7 @@
         <v>93</v>
       </c>
       <c r="G323" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J323" s="0" t="n">
         <v>4</v>
@@ -8428,7 +7641,7 @@
         <v>93</v>
       </c>
       <c r="G324" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J324" s="0" t="n">
         <v>4</v>
@@ -8458,7 +7671,7 @@
         <v>93</v>
       </c>
       <c r="G325" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J325" s="0" t="n">
         <v>4</v>
@@ -8488,7 +7701,7 @@
         <v>93</v>
       </c>
       <c r="G326" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="J326" s="0" t="n">
         <v>4</v>
@@ -8518,7 +7731,7 @@
         <v>93</v>
       </c>
       <c r="G327" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J327" s="0" t="n">
         <v>4</v>
@@ -8578,7 +7791,7 @@
         <v>93</v>
       </c>
       <c r="G329" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J329" s="0" t="n">
         <v>4</v>
@@ -8638,7 +7851,7 @@
         <v>93</v>
       </c>
       <c r="G331" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J331" s="0" t="n">
         <v>4</v>
@@ -8668,7 +7881,7 @@
         <v>93</v>
       </c>
       <c r="G332" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="J332" s="0" t="n">
         <v>4</v>
@@ -8698,7 +7911,7 @@
         <v>93</v>
       </c>
       <c r="G333" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="J333" s="0" t="n">
         <v>4</v>
@@ -8728,7 +7941,7 @@
         <v>93</v>
       </c>
       <c r="G334" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J334" s="0" t="n">
         <v>4</v>
@@ -8758,7 +7971,7 @@
         <v>93</v>
       </c>
       <c r="G335" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J335" s="0" t="n">
         <v>4</v>
@@ -8788,7 +8001,7 @@
         <v>93</v>
       </c>
       <c r="G336" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J336" s="0" t="n">
         <v>4</v>
@@ -8818,7 +8031,7 @@
         <v>93</v>
       </c>
       <c r="G337" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J337" s="0" t="n">
         <v>4</v>
@@ -8848,7 +8061,7 @@
         <v>93</v>
       </c>
       <c r="G338" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J338" s="0" t="n">
         <v>4</v>
@@ -8878,7 +8091,7 @@
         <v>93</v>
       </c>
       <c r="G339" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="J339" s="0" t="n">
         <v>4</v>
@@ -8938,7 +8151,7 @@
         <v>93</v>
       </c>
       <c r="G341" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J341" s="0" t="n">
         <v>4</v>
@@ -8998,7 +8211,7 @@
         <v>93</v>
       </c>
       <c r="G343" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J343" s="0" t="n">
         <v>4</v>
@@ -9058,7 +8271,7 @@
         <v>93</v>
       </c>
       <c r="G345" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="J345" s="0" t="n">
         <v>4</v>
@@ -9088,7 +8301,7 @@
         <v>93</v>
       </c>
       <c r="G346" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J346" s="0" t="n">
         <v>4</v>
@@ -9118,7 +8331,7 @@
         <v>93</v>
       </c>
       <c r="G347" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J347" s="0" t="n">
         <v>4</v>
@@ -9148,7 +8361,7 @@
         <v>93</v>
       </c>
       <c r="G348" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J348" s="0" t="n">
         <v>4</v>
@@ -9178,7 +8391,7 @@
         <v>93</v>
       </c>
       <c r="G349" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J349" s="0" t="n">
         <v>4</v>
@@ -9208,7 +8421,7 @@
         <v>93</v>
       </c>
       <c r="G350" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J350" s="0" t="n">
         <v>4</v>
@@ -9238,7 +8451,7 @@
         <v>93</v>
       </c>
       <c r="G351" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J351" s="0" t="n">
         <v>4</v>
@@ -9256,8 +8469,8 @@
       <c r="E355" s="5"/>
       <c r="F355" s="5"/>
       <c r="G355" s="5"/>
-      <c r="H355" s="5"/>
-      <c r="I355" s="5"/>
+      <c r="H355" s="7"/>
+      <c r="I355" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Major updates to README, and other minor improvements.
</commit_message>
<xml_diff>
--- a/data/geometry_carbonFoam.xlsx
+++ b/data/geometry_carbonFoam.xlsx
@@ -22,31 +22,109 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="13">
   <si>
-    <t xml:space="preserve"> Ring</t>
+    <t xml:space="preserve"> ring</t>
   </si>
   <si>
-    <t xml:space="preserve"> r(mm)</t>
+    <t xml:space="preserve"> r [mm]</t>
   </si>
   <si>
-    <t xml:space="preserve"> phi(deg)</t>
+    <t xml:space="preserve">phi [deg]</t>
   </si>
   <si>
-    <t xml:space="preserve">Relative z [mm]</t>
+    <t xml:space="preserve">relative z [mm]</t>
   </si>
   <si>
-    <t xml:space="preserve">  meanWidth(mm) (orthoradial)</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">  meanWidth </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(orthoradial) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[mm]</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve"> length(mm) (radial)</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">length </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(radial)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> [mm]</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">side</t>
   </si>
   <si>
-    <t xml:space="preserve">insert outer radius (mm) (actual)</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">insert outer radius </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">(actual)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> [mm]</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">insert outer radius (mm)</t>
+    <t xml:space="preserve">insert outer radius [mm]</t>
   </si>
   <si>
     <t xml:space="preserve">radius scale</t>
@@ -70,7 +148,7 @@
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -98,6 +176,17 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -163,7 +252,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -188,43 +277,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L355"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A145" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A180" activeCellId="0" sqref="180:180"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.98"/>
@@ -237,8 +326,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="28.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="32.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="12" style="0" width="8.8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8854,8 +8942,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>